<commit_message>
[rdbms] - remove double-commit scenario to avoid unnecessary error condition. - allow for non-standard or non-CRUD statements.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_rdbms.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_rdbms.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11103"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4D5852-A8B1-6542-8E07-69F7FEC0612B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459FC321-0FF4-6A44-8226-8CABCDCC0973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="35540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -36,10 +36,18 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -49,17 +57,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>true</t>
   </si>
   <si>
-    <t>800</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -75,16 +77,90 @@
     <t>nexial.pollWaitMs</t>
   </si>
   <si>
-    <t>nexial.failFast</t>
-  </si>
-  <si>
-    <t>nexial.textDelim</t>
-  </si>
-  <si>
-    <t>nexial.verbose</t>
-  </si>
-  <si>
-    <t>nexial.openResult</t>
+    <t>0</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/chinook.db</t>
+  </si>
+  <si>
+    <t>dbfile</t>
+  </si>
+  <si>
+    <t>$(syspath|out|fullpath)/test.db</t>
+  </si>
+  <si>
+    <t>testdb-auto.type</t>
+  </si>
+  <si>
+    <t>sqlite</t>
+  </si>
+  <si>
+    <t>testdb-auto.url</t>
+  </si>
+  <si>
+    <t>testdb-auto.autocommit</t>
+  </si>
+  <si>
+    <t>testdb-auto.treatNullAs</t>
+  </si>
+  <si>
+    <t>jdbc:sqlite:${dbfile}</t>
+  </si>
+  <si>
+    <t>&lt;NULL&gt;</t>
+  </si>
+  <si>
+    <t>testdb-manual.type</t>
+  </si>
+  <si>
+    <t>testdb-manual.url</t>
+  </si>
+  <si>
+    <t>testdb-manual.autocommit</t>
+  </si>
+  <si>
+    <t>testdb-manual.treatNullAs</t>
+  </si>
+  <si>
+    <t>golden dbfile</t>
+  </si>
+  <si>
+    <t>sql.test</t>
+  </si>
+  <si>
+    <t>sql.insert.media_types</t>
+  </si>
+  <si>
+    <t>SELECT * FROM media_types;</t>
+  </si>
+  <si>
+    <t>INSERT INTO media_types VALUES (1000,'XYZ');</t>
+  </si>
+  <si>
+    <t>sql.batch</t>
+  </si>
+  <si>
+    <t>DELETE FROM media_types WHERE mediatypeid = 1000;
+INSERT INTO media_types VALUES (2000,'ABC');
+INSERT INTO media_types VALUES (2001,'EFG');
+COMMIT;
+SELECT * FROM media_types;</t>
+  </si>
+  <si>
+    <t>sql.delete.media_types</t>
+  </si>
+  <si>
+    <t>DELETE FROM media_types WHERE mediatypeid &gt;= 1000;</t>
+  </si>
+  <si>
+    <t>sql.batch2</t>
+  </si>
+  <si>
+    <t>DELETE FROM media_types WHERE mediatypeid = 1000;
+INSERT INTO media_types VALUES (2002,'ABC');
+INSERT INTO media_types VALUES (2003,'EFG');
+ROLLBACK;
+SELECT * FROM media_types;</t>
   </si>
 </sst>
 </file>
@@ -152,7 +228,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -175,6 +251,135 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </right>
+      <top style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </left>
+      <right style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </right>
+      <top style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </left>
+      <right style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </right>
+      <top style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </right>
+      <top style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color theme="6" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
@@ -187,7 +392,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -217,6 +422,54 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -600,19 +853,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="54.5703125" style="4" customWidth="1" collapsed="1"/>
     <col min="3" max="52" width="21.28515625" style="2" customWidth="1" collapsed="1"/>
     <col min="53" max="16384" width="10.7109375" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -622,143 +877,206 @@
     </row>
     <row r="2" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="HA2" s="3"/>
       <c r="AAA2" s="3"/>
     </row>
     <row r="3" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="HA3" s="3"/>
       <c r="AAA3" s="3"/>
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="HA4" s="6"/>
       <c r="AAA4" s="7"/>
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>2</v>
       </c>
       <c r="HA5" s="6"/>
       <c r="AAA5" s="7"/>
     </row>
     <row r="6" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="B6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="8"/>
       <c r="HA6" s="6"/>
       <c r="AAA6" s="7"/>
     </row>
     <row r="7" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="A7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="8"/>
       <c r="HA7" s="6"/>
       <c r="AAA7" s="7"/>
     </row>
     <row r="8" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8"/>
       <c r="HA8" s="6"/>
       <c r="AAA8" s="7"/>
     </row>
     <row r="9" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="8"/>
       <c r="HA9" s="6"/>
       <c r="AAA9" s="7"/>
     </row>
     <row r="10" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="8"/>
       <c r="HA10" s="6"/>
       <c r="AAA10" s="7"/>
     </row>
     <row r="11" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="8"/>
     </row>
     <row r="14" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:703" ht="144" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="149" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -1266,7 +1584,7 @@
       <c r="A200" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="beginsWith" dxfId="5" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>

</xml_diff>

<commit_message>
[rdbms] - fixed error when handling the execution of stored procedures which might contain multiple results (result set and   possibly update row count). - for executing stored procedure, both the `{CALL ...(...)}` and `EXEC ... ...` forms are supported now.
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_rdbms.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_rdbms.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11103"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\nexial\nexial-core\src\test\resources\unittesting\artifact\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459FC321-0FF4-6A44-8226-8CABCDCC0973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C43945-BFFC-4B66-A82A-E263878D758B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="35540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="-14880" windowWidth="27420" windowHeight="4845" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -44,9 +44,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -57,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>true</t>
   </si>
@@ -161,6 +159,9 @@
 INSERT INTO media_types VALUES (2003,'EFG');
 ROLLBACK;
 SELECT * FROM media_types;</t>
+  </si>
+  <si>
+    <t>nexial.delayBetweenStepsMs</t>
   </si>
 </sst>
 </file>
@@ -514,19 +515,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <color theme="1"/>
@@ -559,6 +547,19 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -851,21 +852,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA200"/>
+  <dimension ref="A1:AAA201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="52" width="21.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="53" max="16384" width="10.7109375" style="2" collapsed="1"/>
+    <col min="1" max="1" width="23.69921875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="51.8984375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="52" width="21.296875" style="2" customWidth="1" collapsed="1"/>
+    <col min="53" max="16384" width="10.69921875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -875,7 +876,7 @@
       <c r="HA1" s="3"/>
       <c r="AAA1" s="3"/>
     </row>
-    <row r="2" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -885,9 +886,9 @@
       <c r="HA2" s="3"/>
       <c r="AAA2" s="3"/>
     </row>
-    <row r="3" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
@@ -895,708 +896,718 @@
       <c r="HA3" s="3"/>
       <c r="AAA3" s="3"/>
     </row>
-    <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="HA4" s="3"/>
+      <c r="AAA4" s="3"/>
+    </row>
+    <row r="5" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="HA4" s="6"/>
-      <c r="AAA4" s="7"/>
-    </row>
-    <row r="5" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>9</v>
       </c>
       <c r="HA5" s="6"/>
       <c r="AAA5" s="7"/>
     </row>
-    <row r="6" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="8"/>
+    <row r="6" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="HA6" s="6"/>
       <c r="AAA6" s="7"/>
     </row>
-    <row r="7" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>15</v>
+    <row r="7" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="C7" s="8"/>
       <c r="HA7" s="6"/>
       <c r="AAA7" s="7"/>
     </row>
-    <row r="8" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C8" s="8"/>
       <c r="HA8" s="6"/>
       <c r="AAA8" s="7"/>
     </row>
-    <row r="9" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>16</v>
+    <row r="9" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>0</v>
       </c>
       <c r="C9" s="8"/>
       <c r="HA9" s="6"/>
       <c r="AAA9" s="7"/>
     </row>
-    <row r="10" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>11</v>
+    <row r="10" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="C10" s="8"/>
       <c r="HA10" s="6"/>
       <c r="AAA10" s="7"/>
     </row>
-    <row r="11" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+    <row r="11" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="HA11" s="6"/>
+      <c r="AAA11" s="7"/>
+    </row>
+    <row r="12" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B12" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B13" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B14" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B15" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:703" ht="144" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:2" ht="126" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B17" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B18" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="149" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:2" ht="149.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B19" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:2" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
     </row>
-    <row r="65" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
     </row>
-    <row r="76" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
     </row>
-    <row r="77" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
     </row>
-    <row r="81" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
     </row>
-    <row r="82" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
     </row>
-    <row r="83" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
     </row>
-    <row r="84" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
     </row>
-    <row r="85" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
     </row>
-    <row r="86" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
     </row>
-    <row r="87" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
     </row>
-    <row r="88" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
     </row>
-    <row r="89" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
     </row>
-    <row r="90" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
     </row>
-    <row r="91" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
     </row>
-    <row r="92" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
     </row>
-    <row r="93" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
     </row>
-    <row r="94" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
     </row>
-    <row r="95" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
     </row>
-    <row r="98" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
     </row>
-    <row r="100" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
     </row>
-    <row r="101" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
     </row>
-    <row r="102" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
     </row>
-    <row r="103" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
     </row>
-    <row r="104" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
     </row>
-    <row r="105" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
     </row>
-    <row r="106" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
     </row>
-    <row r="107" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
     </row>
-    <row r="108" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
     </row>
-    <row r="109" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
     </row>
-    <row r="111" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
     </row>
-    <row r="112" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
     </row>
-    <row r="113" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
     </row>
-    <row r="114" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
     </row>
-    <row r="115" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
     </row>
-    <row r="116" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
     </row>
-    <row r="117" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
     </row>
-    <row r="118" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
     </row>
-    <row r="119" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
     </row>
-    <row r="120" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
     </row>
-    <row r="121" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
     </row>
-    <row r="122" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
     </row>
-    <row r="123" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
     </row>
-    <row r="124" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
     </row>
-    <row r="129" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
     </row>
-    <row r="130" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
     </row>
-    <row r="131" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
     </row>
-    <row r="132" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
     </row>
-    <row r="133" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
     </row>
-    <row r="134" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
     </row>
-    <row r="135" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
     </row>
-    <row r="136" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
     </row>
-    <row r="137" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
     </row>
-    <row r="138" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
     </row>
-    <row r="139" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
     </row>
-    <row r="140" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
     </row>
-    <row r="141" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
     </row>
-    <row r="142" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
     </row>
-    <row r="143" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
     </row>
-    <row r="144" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
     </row>
-    <row r="145" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
     </row>
-    <row r="146" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
     </row>
-    <row r="147" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
     </row>
-    <row r="148" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
     </row>
-    <row r="149" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
     </row>
-    <row r="150" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
     </row>
-    <row r="151" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
     </row>
-    <row r="152" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
     </row>
-    <row r="153" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
     </row>
-    <row r="154" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
     </row>
-    <row r="155" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
     </row>
-    <row r="156" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
     </row>
-    <row r="157" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
     </row>
-    <row r="158" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
     </row>
-    <row r="159" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
     </row>
-    <row r="160" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
     </row>
-    <row r="161" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
     </row>
-    <row r="162" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
     </row>
-    <row r="163" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
     </row>
-    <row r="164" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
     </row>
-    <row r="165" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
     </row>
-    <row r="166" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
     </row>
-    <row r="167" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
     </row>
-    <row r="168" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
     </row>
-    <row r="169" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
     </row>
-    <row r="170" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
     </row>
-    <row r="171" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
     </row>
-    <row r="172" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
     </row>
-    <row r="173" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
     </row>
-    <row r="174" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
     </row>
-    <row r="175" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
     </row>
-    <row r="176" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
     </row>
-    <row r="177" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
     </row>
-    <row r="178" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
     </row>
-    <row r="179" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
     </row>
-    <row r="180" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
     </row>
-    <row r="181" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
     </row>
-    <row r="182" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
     </row>
-    <row r="183" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
     </row>
-    <row r="184" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
     </row>
-    <row r="185" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
     </row>
-    <row r="186" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
     </row>
-    <row r="187" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
     </row>
-    <row r="188" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
     </row>
-    <row r="189" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
     </row>
-    <row r="190" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
     </row>
-    <row r="191" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
     </row>
-    <row r="192" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
     </row>
-    <row r="193" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
     </row>
-    <row r="194" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
     </row>
-    <row r="195" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
     </row>
-    <row r="196" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
     </row>
-    <row r="197" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
     </row>
-    <row r="198" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
     </row>
-    <row r="199" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
     </row>
-    <row r="200" spans="1:1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
+    </row>
+    <row r="201" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="5" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="5" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
+      <formula>LEFT(A1,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="4" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="3" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="//">
-      <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:AZ1048576">

</xml_diff>